<commit_message>
python and ui changes
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,191 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Expertise</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Organization</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Onshore/Offshore</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Resource Manager</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Rate</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Feb'23</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Mar'23</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Apr'23</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>May'23</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Jun'23</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Jul'23</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Aug'23</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Sept'23</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Oct'23</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Nov'23</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Dec'23</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Jan'24</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Feb'24</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Mar'24</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Total Hours</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Total Amount</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Test Lead</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Kamalesh D</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>VSIT</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Onshore</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ram</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>435</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>454</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>4354</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>